<commit_message>
updated planning for events
</commit_message>
<xml_diff>
--- a/Planning/RandomEvent.xlsx
+++ b/Planning/RandomEvent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RandomCreation\project\DSELife\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3307761-A60E-4668-B82C-037D490A1B43}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ABCAD0-771A-4DE3-A70B-87994D2A525C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="1155" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>Condition</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,6 +84,94 @@
   </si>
   <si>
     <t>Suicide</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Classmate remind for break </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy &lt; 30 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Frequency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Random</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Always</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only in first time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Borrow money</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Borrow money from classmate </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Money &lt; 100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remind user that may not have enough money for tutorial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remind user that they may have to borrow money</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Money &gt; 1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classmate help for tutorial but need to pay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific subject + 20 in knowledge and examSkill, money - 600                           </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Random -small chance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classmate laugh at player</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Break for whole day due to unhappiness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classmate remind that if tired for many times, may exhaust</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same subject tired</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classmate remind that don't study same subject for whole day</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -127,10 +215,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,35 +503,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="57.42578125" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="35.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -450,90 +545,241 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="E11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E15" s="2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set up file structure for event system
</commit_message>
<xml_diff>
--- a/Planning/RandomEvent.xlsx
+++ b/Planning/RandomEvent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RandomCreation\project\DSELife\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ABCAD0-771A-4DE3-A70B-87994D2A525C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EBD4E3-354A-44BB-A268-E2624D27DEEE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>Condition</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -173,6 +173,47 @@
   <si>
     <t>Classmate remind that don't study same subject for whole day</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tired_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tired_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tired_3</t>
+  </si>
+  <si>
+    <t>exhaust_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exhaust_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>energy_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>money_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>money_2</t>
+  </si>
+  <si>
+    <t>money_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>money_4</t>
   </si>
 </sst>
 </file>
@@ -503,282 +544,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="48.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="35.28515625" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3"/>
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+      <c r="E3"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="C4"/>
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4"/>
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5"/>
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5"/>
+      <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9"/>
+      <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
+      <c r="E9"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C10"/>
+      <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10"/>
+      <c r="F10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11"/>
+      <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11"/>
+      <c r="F11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13"/>
+      <c r="D13" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
+      <c r="E13"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C14"/>
+      <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14"/>
+      <c r="F14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15"/>
+      <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15"/>
+      <c r="F15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
       <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
       <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8</v>
       </c>
       <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
+    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C19"/>
+      <c r="D19" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E19"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
       <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
       <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="2" t="s">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22"/>
+      <c r="D22" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C23" s="2" t="s">
+      <c r="E22"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="126" x14ac:dyDescent="0.25">
+      <c r="C23"/>
+      <c r="D23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23"/>
+      <c r="F23" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="2" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24"/>
+      <c r="D24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24"/>
+      <c r="F24" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implement text of underStory
</commit_message>
<xml_diff>
--- a/Planning/RandomEvent.xlsx
+++ b/Planning/RandomEvent.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RandomCreation\project\DSELife\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFD9B58-634D-466C-A2CB-EC2CC4FED2D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3BFAFA-1886-4EBE-A1C4-092C75477C79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="90">
   <si>
     <t>Condition</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -217,6 +217,157 @@
   </si>
   <si>
     <t xml:space="preserve">All subject + 20 in knowledge and examSkill, money - 600                           </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>understory1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>understory2</t>
+  </si>
+  <si>
+    <t>understory3</t>
+  </si>
+  <si>
+    <t>understory4</t>
+  </si>
+  <si>
+    <t>understory5</t>
+  </si>
+  <si>
+    <t>understory6</t>
+  </si>
+  <si>
+    <t>understory7</t>
+  </si>
+  <si>
+    <t>understory8</t>
+  </si>
+  <si>
+    <t>understory9</t>
+  </si>
+  <si>
+    <t>substory1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>substory2</t>
+  </si>
+  <si>
+    <t>substory3</t>
+  </si>
+  <si>
+    <t>substory4</t>
+  </si>
+  <si>
+    <t>substory5</t>
+  </si>
+  <si>
+    <t>substory6</t>
+  </si>
+  <si>
+    <t>Day 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day 9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day 30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day 27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day 14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day 24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Choose 'ask' in understory5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Choose 'not ask' in understory5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Choose 'back home' in understory7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Choose 'find teacher' in understory7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Choose 'go' in understory8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Choose 'don't go' in understory8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Ask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.Not ask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Back home</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.Find teacher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>substory3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>substory4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Go</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.Don't go</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>substory5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>substory6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>End game</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -548,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -896,6 +1047,361 @@
         <v>9</v>
       </c>
     </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>19</v>
+      </c>
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>20</v>
+      </c>
+      <c r="B43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>21</v>
+      </c>
+      <c r="B44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>23</v>
+      </c>
+      <c r="B46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>24</v>
+      </c>
+      <c r="B47" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>25</v>
+      </c>
+      <c r="B48" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add picture of underStory1
</commit_message>
<xml_diff>
--- a/Planning/RandomEvent.xlsx
+++ b/Planning/RandomEvent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RandomCreation\project\DSELife\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3BFAFA-1886-4EBE-A1C4-092C75477C79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34493D4A-3549-413D-B2F5-5068A23DB1AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9585" yWindow="765" windowWidth="9495" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="92">
   <si>
     <t>Condition</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -368,6 +368,13 @@
   </si>
   <si>
     <t>End game</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>understory10</t>
+  </si>
+  <si>
+    <t>Day 16</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -699,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1181,7 @@
         <v>54</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
         <v>54</v>
@@ -1194,7 +1201,7 @@
         <v>55</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D34" t="s">
         <v>55</v>
@@ -1232,7 +1239,7 @@
         <v>56</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D38" t="s">
         <v>56</v>
@@ -1270,7 +1277,7 @@
         <v>57</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D42" t="s">
         <v>57</v>
@@ -1287,13 +1294,13 @@
         <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>19</v>
@@ -1307,13 +1314,13 @@
         <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>19</v>
@@ -1327,13 +1334,13 @@
         <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>19</v>
@@ -1347,13 +1354,13 @@
         <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>19</v>
@@ -1367,19 +1374,19 @@
         <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F47" t="s">
-        <v>89</v>
+      <c r="F47" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1387,18 +1394,38 @@
         <v>25</v>
       </c>
       <c r="B48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" t="s">
+        <v>62</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>26</v>
+      </c>
+      <c r="B49" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>63</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="2" t="s">
+      <c r="E49" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>